<commit_message>
Finalização do estudo básico de pandas
Finalização do estudo de Pandas, foi criado o arquivo "ConsolidadoPandas" Para seguir os estudos apresentados no canal do 'Xavecoding'
</commit_message>
<xml_diff>
--- a/Python/teste/Organizacao.xlsx
+++ b/Python/teste/Organizacao.xlsx
@@ -5,16 +5,16 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevyn\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevyn\Documents\Main_repository\Python\teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBECEE1-D43D-4CC0-B7BB-1E9F03007401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34802CBE-1E2B-4391-BCCD-5A912F70B40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{0AFBF572-1A46-4E4A-8041-A4CE242F5D0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Resumo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -251,15 +251,15 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -680,94 +680,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="E1" s="7"/>
+      <c r="H1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="I1" s="7"/>
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="L1" s="7"/>
+      <c r="N1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="O1" s="7"/>
+      <c r="Q1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="T1" s="1" t="s">
+      <c r="R1" s="7"/>
+      <c r="T1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1"/>
-      <c r="W1" s="1" t="s">
+      <c r="U1" s="7"/>
+      <c r="W1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1"/>
-      <c r="Z1" s="1" t="s">
+      <c r="X1" s="7"/>
+      <c r="Z1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="1"/>
-      <c r="AC1" s="1" t="s">
+      <c r="AA1" s="7"/>
+      <c r="AC1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="1"/>
-      <c r="AF1" s="1" t="s">
+      <c r="AD1" s="7"/>
+      <c r="AF1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="1"/>
-      <c r="AI1" s="1" t="s">
+      <c r="AG1" s="7"/>
+      <c r="AI1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" s="1"/>
-      <c r="AL1" s="1" t="s">
+      <c r="AJ1" s="7"/>
+      <c r="AL1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="1"/>
-      <c r="AO1" s="1" t="s">
+      <c r="AM1" s="7"/>
+      <c r="AO1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AP1" s="1"/>
-      <c r="AR1" s="1" t="s">
+      <c r="AP1" s="7"/>
+      <c r="AR1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AS1" s="1"/>
-      <c r="AU1" s="1" t="s">
+      <c r="AS1" s="7"/>
+      <c r="AU1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AV1" s="1"/>
-      <c r="AX1" s="1" t="s">
+      <c r="AV1" s="7"/>
+      <c r="AX1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AY1" s="1"/>
-      <c r="BA1" s="1" t="s">
+      <c r="AY1" s="7"/>
+      <c r="BA1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="BB1" s="1"/>
-      <c r="BD1" s="1" t="s">
+      <c r="BB1" s="7"/>
+      <c r="BD1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="BE1" s="1"/>
-      <c r="BG1" s="1" t="s">
+      <c r="BE1" s="7"/>
+      <c r="BG1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="BH1" s="1"/>
-      <c r="BJ1" s="1" t="s">
+      <c r="BH1" s="7"/>
+      <c r="BJ1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="BK1" s="1"/>
-      <c r="BM1" s="1" t="s">
+      <c r="BK1" s="7"/>
+      <c r="BM1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="BN1" s="1"/>
+      <c r="BN1" s="7"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1578,10 +1578,10 @@
       </c>
     </row>
     <row r="11" spans="1:66" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="7"/>
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1590,10 +1590,10 @@
       <c r="B12">
         <v>255</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1">
         <v>2000</v>
       </c>
       <c r="G12" t="s">
@@ -1610,10 +1610,10 @@
       <c r="B13">
         <v>500</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <f>H17</f>
         <v>576</v>
       </c>
@@ -1631,10 +1631,10 @@
       <c r="B14">
         <v>122.5</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <f>H19</f>
         <v>327.56</v>
       </c>
@@ -1654,10 +1654,10 @@
         <f>7.5 * 15</f>
         <v>112.5</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <f>E12-E13-E14</f>
         <v>1096.44</v>
       </c>
@@ -1725,17 +1725,6 @@
   </scenarios>
   <dataConsolidate/>
   <mergeCells count="23">
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="BM1:BN1"/>
     <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="AI1:AJ1"/>
@@ -1748,6 +1737,17 @@
     <mergeCell ref="BD1:BE1"/>
     <mergeCell ref="BG1:BH1"/>
     <mergeCell ref="BJ1:BK1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1780,37 +1780,37 @@
       <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1818,37 +1818,37 @@
       <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>1249.78</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <v>1250.78</v>
       </c>
     </row>
@@ -1856,47 +1856,47 @@
       <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>766.46</v>
       </c>
-      <c r="D5" s="3">
-        <f>C14</f>
+      <c r="D5" s="2">
+        <f t="shared" ref="D5:M5" si="0">C14</f>
         <v>873.69</v>
       </c>
-      <c r="E5" s="3">
-        <f>D14</f>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
         <v>947.8599999999999</v>
       </c>
-      <c r="F5" s="3">
-        <f>E14</f>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
         <v>1324.1399999999999</v>
       </c>
-      <c r="G5" s="3">
-        <f>F14</f>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
         <v>2360.42</v>
       </c>
-      <c r="H5" s="3">
-        <f>G14</f>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
         <v>3396.7</v>
       </c>
-      <c r="I5" s="3">
-        <f>H14</f>
+      <c r="I5" s="2">
+        <f t="shared" si="0"/>
         <v>4432.9799999999996</v>
       </c>
-      <c r="J5" s="3">
-        <f>I14</f>
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
         <v>5469.2599999999993</v>
       </c>
-      <c r="K5" s="3">
-        <f>J14</f>
+      <c r="K5" s="2">
+        <f t="shared" si="0"/>
         <v>6505.5399999999991</v>
       </c>
-      <c r="L5" s="3">
-        <f>K14</f>
+      <c r="L5" s="2">
+        <f t="shared" si="0"/>
         <v>7541.8199999999988</v>
       </c>
-      <c r="M5" s="3">
-        <f>L14</f>
+      <c r="M5" s="2">
+        <f t="shared" si="0"/>
         <v>8578.0999999999985</v>
       </c>
     </row>
@@ -1904,37 +1904,37 @@
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>255</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>255</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>255</v>
       </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0</v>
-      </c>
-      <c r="M6" s="3">
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1942,37 +1942,37 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>122.5</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>122.5</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>122.5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>122.5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>122.5</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>122.5</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>122.5</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>122.5</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>122.5</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>122.5</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="2">
         <v>122.5</v>
       </c>
     </row>
@@ -1980,48 +1980,48 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <f>7 * 15</f>
         <v>105</v>
       </c>
-      <c r="D8" s="3">
-        <f t="shared" ref="D8:M8" si="0">7 * 15</f>
+      <c r="D8" s="2">
+        <f t="shared" ref="D8:M8" si="1">7 * 15</f>
         <v>105</v>
       </c>
-      <c r="E8" s="3">
-        <f t="shared" si="0"/>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="F8" s="3">
-        <f t="shared" si="0"/>
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="G8" s="3">
-        <f t="shared" si="0"/>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="H8" s="3">
-        <f t="shared" si="0"/>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="I8" s="3">
-        <f t="shared" si="0"/>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="J8" s="3">
-        <f t="shared" si="0"/>
+      <c r="J8" s="2">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="K8" s="3">
-        <f t="shared" si="0"/>
+      <c r="K8" s="2">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="L8" s="3">
-        <f t="shared" si="0"/>
+      <c r="L8" s="2">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="M8" s="3">
-        <f t="shared" si="0"/>
+      <c r="M8" s="2">
+        <f t="shared" si="1"/>
         <v>105</v>
       </c>
     </row>
@@ -2029,48 +2029,48 @@
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="D9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="E9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="F9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="G9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="H9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="I9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="J9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="K9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="L9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
-        <v>36</v>
-      </c>
-      <c r="M9" s="3">
-        <f xml:space="preserve"> (4.5 *2) *4</f>
+      <c r="C9" s="2">
+        <f t="shared" ref="C9:M9" si="2" xml:space="preserve"> (4.5 *2) *4</f>
+        <v>36</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
     </row>
@@ -2078,37 +2078,37 @@
       <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>327.56</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>707.11</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>405</v>
       </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3">
-        <v>0</v>
-      </c>
-      <c r="M10" s="3">
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2116,38 +2116,38 @@
       <c r="B11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <f>113.47+30.5+8+134.18+4.46+23.46+23.5+8.92</f>
         <v>346.48999999999995</v>
       </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0</v>
-      </c>
-      <c r="M11" s="5">
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2155,37 +2155,37 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>50</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>50</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>50</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>50</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>50</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>50</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>50</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>50</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="2">
         <v>50</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="2">
         <v>50</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12" s="2">
         <v>50</v>
       </c>
     </row>
@@ -2193,48 +2193,48 @@
       <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <f>C4-SUM(C6:C11)</f>
         <v>57.230000000000018</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <f>D4-SUM(D6:D11)</f>
         <v>24.169999999999845</v>
       </c>
-      <c r="E13" s="3">
-        <f t="shared" ref="E13:M13" si="1">E4-SUM(E6:E11)</f>
+      <c r="E13" s="2">
+        <f t="shared" ref="E13:M13" si="3">E4-SUM(E6:E11)</f>
         <v>326.27999999999997</v>
       </c>
-      <c r="F13" s="3">
-        <f t="shared" si="1"/>
+      <c r="F13" s="2">
+        <f t="shared" si="3"/>
         <v>986.28</v>
       </c>
-      <c r="G13" s="3">
-        <f t="shared" si="1"/>
+      <c r="G13" s="2">
+        <f t="shared" si="3"/>
         <v>986.28</v>
       </c>
-      <c r="H13" s="3">
-        <f t="shared" si="1"/>
+      <c r="H13" s="2">
+        <f t="shared" si="3"/>
         <v>986.28</v>
       </c>
-      <c r="I13" s="3">
-        <f t="shared" si="1"/>
+      <c r="I13" s="2">
+        <f t="shared" si="3"/>
         <v>986.28</v>
       </c>
-      <c r="J13" s="3">
-        <f t="shared" si="1"/>
+      <c r="J13" s="2">
+        <f t="shared" si="3"/>
         <v>986.28</v>
       </c>
-      <c r="K13" s="3">
-        <f t="shared" si="1"/>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
         <v>986.28</v>
       </c>
-      <c r="L13" s="3">
-        <f t="shared" si="1"/>
+      <c r="L13" s="2">
+        <f t="shared" si="3"/>
         <v>986.28</v>
       </c>
-      <c r="M13" s="3">
-        <f t="shared" si="1"/>
+      <c r="M13" s="2">
+        <f t="shared" si="3"/>
         <v>987.28</v>
       </c>
     </row>
@@ -2245,48 +2245,48 @@
       <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="3">
-        <f>SUM(C5,C12,C13)</f>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14:M14" si="4">SUM(C5,C12,C13)</f>
         <v>873.69</v>
       </c>
-      <c r="D14" s="3">
-        <f>SUM(D5,D12,D13)</f>
+      <c r="D14" s="2">
+        <f t="shared" si="4"/>
         <v>947.8599999999999</v>
       </c>
-      <c r="E14" s="3">
-        <f>SUM(E5,E12,E13)</f>
+      <c r="E14" s="2">
+        <f t="shared" si="4"/>
         <v>1324.1399999999999</v>
       </c>
-      <c r="F14" s="3">
-        <f>SUM(F5,F12,F13)</f>
+      <c r="F14" s="2">
+        <f t="shared" si="4"/>
         <v>2360.42</v>
       </c>
-      <c r="G14" s="3">
-        <f>SUM(G5,G12,G13)</f>
+      <c r="G14" s="2">
+        <f t="shared" si="4"/>
         <v>3396.7</v>
       </c>
-      <c r="H14" s="3">
-        <f>SUM(H5,H12,H13)</f>
+      <c r="H14" s="2">
+        <f t="shared" si="4"/>
         <v>4432.9799999999996</v>
       </c>
-      <c r="I14" s="3">
-        <f>SUM(I5,I12,I13)</f>
+      <c r="I14" s="2">
+        <f t="shared" si="4"/>
         <v>5469.2599999999993</v>
       </c>
-      <c r="J14" s="3">
-        <f>SUM(J5,J12,J13)</f>
+      <c r="J14" s="2">
+        <f t="shared" si="4"/>
         <v>6505.5399999999991</v>
       </c>
-      <c r="K14" s="3">
-        <f>SUM(K5,K12,K13)</f>
+      <c r="K14" s="2">
+        <f t="shared" si="4"/>
         <v>7541.8199999999988</v>
       </c>
-      <c r="L14" s="3">
-        <f>SUM(L5,L12,L13)</f>
+      <c r="L14" s="2">
+        <f t="shared" si="4"/>
         <v>8578.0999999999985</v>
       </c>
-      <c r="M14" s="3">
-        <f>SUM(M5,M12,M13)</f>
+      <c r="M14" s="2">
+        <f t="shared" si="4"/>
         <v>9615.3799999999992</v>
       </c>
     </row>
@@ -2297,58 +2297,58 @@
       <c r="B15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <f>(C12/$A$15)</f>
         <v>8.5470085470085468</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f>(D12/$A$15) +Tabela1[[#This Row],[Fevereiro]]</f>
         <v>17.094017094017094</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <f>(E12/$A$15) +Tabela1[[#This Row],[Março]]</f>
         <v>25.641025641025642</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <f>(F12/$A$15) +Tabela1[[#This Row],[Abril]]</f>
         <v>34.188034188034187</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <f>(G12/$A$15) +Tabela1[[#This Row],[Maio]]</f>
         <v>42.735042735042732</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <f>(H12/$A$15) +Tabela1[[#This Row],[Junho]]</f>
         <v>51.282051282051277</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <f>(I12/$A$15) +Tabela1[[#This Row],[Julho]]</f>
         <v>59.829059829059823</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <f>(J12/$A$15) +Tabela1[[#This Row],[Agosto]]</f>
         <v>68.376068376068375</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <f>(K12/$A$15) +Tabela1[[#This Row],[Setembro]]</f>
         <v>76.92307692307692</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="3">
         <f>(L12/$A$15) +Tabela1[[#This Row],[Outubro]]</f>
         <v>85.470085470085465</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="3">
         <f>(M12/$A$15) +Tabela1[[#This Row],[Novembro]]</f>
         <v>94.01709401709401</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C16" s="4"/>
+      <c r="C16" s="3"/>
     </row>
   </sheetData>
   <dataConsolidate>
     <dataRefs count="1">
-      <dataRef ref="C14:M14" sheet="Planilha2"/>
+      <dataRef ref="C14:M14" sheet="Resumo"/>
     </dataRefs>
   </dataConsolidate>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Estudo sobre bibliotecas de Análise de dados e organização
Foi feito o estudo do essencial da biblioteca pandas, numpy, e um pouco de matplotlib. Foram excluídos os arquivos referentes as bibliotecas Seaborn, plotly, Dash, streamlit e foram adicionados os arquivos pertinentes aos estudos das primeiras bibliotecas
</commit_message>
<xml_diff>
--- a/Python/teste/Organizacao.xlsx
+++ b/Python/teste/Organizacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevyn\Documents\Main_repository\Python\teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34802CBE-1E2B-4391-BCCD-5A912F70B40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C067689-AA8F-4346-8D2B-ADFF8A8333BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{0AFBF572-1A46-4E4A-8041-A4CE242F5D0A}"/>
   </bookViews>
@@ -1725,6 +1725,17 @@
   </scenarios>
   <dataConsolidate/>
   <mergeCells count="23">
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="BM1:BN1"/>
     <mergeCell ref="AF1:AG1"/>
     <mergeCell ref="AI1:AJ1"/>
@@ -1737,17 +1748,6 @@
     <mergeCell ref="BD1:BE1"/>
     <mergeCell ref="BG1:BH1"/>
     <mergeCell ref="BJ1:BK1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1760,7 +1760,7 @@
   <dimension ref="A3:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1873,31 +1873,31 @@
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>2360.42</v>
+        <v>2560.42</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>3396.7</v>
+        <v>3796.7</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>4432.9799999999996</v>
+        <v>5032.9799999999996</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>5469.2599999999993</v>
+        <v>6269.2599999999993</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="0"/>
-        <v>6505.5399999999991</v>
+        <v>7505.5399999999991</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" si="0"/>
-        <v>7541.8199999999988</v>
+        <v>8741.82</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" si="0"/>
-        <v>8578.0999999999985</v>
+        <v>9978.1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -2165,28 +2165,28 @@
         <v>50</v>
       </c>
       <c r="F12" s="2">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="G12" s="2">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="H12" s="2">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="I12" s="2">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="J12" s="2">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="K12" s="2">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="L12" s="2">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="M12" s="2">
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -2259,87 +2259,87 @@
       </c>
       <c r="F14" s="2">
         <f t="shared" si="4"/>
-        <v>2360.42</v>
+        <v>2560.42</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="4"/>
-        <v>3396.7</v>
+        <v>3796.7</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="4"/>
-        <v>4432.9799999999996</v>
+        <v>5032.9799999999996</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="4"/>
-        <v>5469.2599999999993</v>
+        <v>6269.2599999999993</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="4"/>
-        <v>6505.5399999999991</v>
+        <v>7505.5399999999991</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="4"/>
-        <v>7541.8199999999988</v>
+        <v>8741.82</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" si="4"/>
-        <v>8578.0999999999985</v>
+        <v>9978.1</v>
       </c>
       <c r="M14" s="2">
         <f t="shared" si="4"/>
-        <v>9615.3799999999992</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+        <v>11215.380000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>5.85</v>
+        <v>5.64</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
       </c>
       <c r="C15" s="3">
         <f>(C12/$A$15)</f>
-        <v>8.5470085470085468</v>
+        <v>8.8652482269503547</v>
       </c>
       <c r="D15" s="3">
         <f>(D12/$A$15) +Tabela1[[#This Row],[Fevereiro]]</f>
-        <v>17.094017094017094</v>
+        <v>17.730496453900709</v>
       </c>
       <c r="E15" s="3">
         <f>(E12/$A$15) +Tabela1[[#This Row],[Março]]</f>
-        <v>25.641025641025642</v>
+        <v>26.595744680851062</v>
       </c>
       <c r="F15" s="3">
         <f>(F12/$A$15) +Tabela1[[#This Row],[Abril]]</f>
-        <v>34.188034188034187</v>
+        <v>70.921985815602838</v>
       </c>
       <c r="G15" s="3">
         <f>(G12/$A$15) +Tabela1[[#This Row],[Maio]]</f>
-        <v>42.735042735042732</v>
+        <v>115.24822695035462</v>
       </c>
       <c r="H15" s="3">
         <f>(H12/$A$15) +Tabela1[[#This Row],[Junho]]</f>
-        <v>51.282051282051277</v>
+        <v>159.57446808510639</v>
       </c>
       <c r="I15" s="3">
         <f>(I12/$A$15) +Tabela1[[#This Row],[Julho]]</f>
-        <v>59.829059829059823</v>
+        <v>203.90070921985816</v>
       </c>
       <c r="J15" s="3">
         <f>(J12/$A$15) +Tabela1[[#This Row],[Agosto]]</f>
-        <v>68.376068376068375</v>
+        <v>248.22695035460993</v>
       </c>
       <c r="K15" s="3">
         <f>(K12/$A$15) +Tabela1[[#This Row],[Setembro]]</f>
-        <v>76.92307692307692</v>
+        <v>292.55319148936172</v>
       </c>
       <c r="L15" s="3">
         <f>(L12/$A$15) +Tabela1[[#This Row],[Outubro]]</f>
-        <v>85.470085470085465</v>
+        <v>336.87943262411352</v>
       </c>
       <c r="M15" s="3">
         <f>(M12/$A$15) +Tabela1[[#This Row],[Novembro]]</f>
-        <v>94.01709401709401</v>
+        <v>381.20567375886532</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>